<commit_message>
customize Template for transaction in form of json from folder
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicos\Git\RPATestingGetOrdersBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412CA73D-CEC9-426B-8BC6-C4C1A529D335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -88,20 +88,12 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -120,12 +112,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
     <t>MaxConsecutiveSystemExceptions</t>
   </si>
   <si>
@@ -159,7 +145,10 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>inputFolder</t>
+  </si>
+  <si>
+    <t>Data/Input</t>
   </si>
 </sst>
 </file>
@@ -211,11 +200,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -223,7 +211,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,7 +227,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -535,18 +523,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -583,38 +571,27 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:26" ht="29">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1605,9 +1582,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1623,12 +1597,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,26 +1639,26 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>25</v>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>41</v>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1682,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1704,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1715,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1726,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>42</v>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,14 +2756,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
add Log Messages and move file to Folder before BE
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicos\Git\RPATestingGetOrdersBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F85FBF0-B1BA-4D2E-9172-8F9D2D4FF45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47B5AC3-819A-4735-8307-E5E6776EEB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="230" yWindow="220" windowWidth="28710" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>out_Folder_Success</t>
+  </si>
+  <si>
+    <t>out_Folder_BE</t>
+  </si>
+  <si>
+    <t>Data/Output_BE</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -629,7 +635,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add lasttest with random data
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicos\Git\RPATestingGetOrdersBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47B5AC3-819A-4735-8307-E5E6776EEB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D125FA-FD51-4A0F-AA56-7B059AF64EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="230" yWindow="220" windowWidth="28710" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7830" yWindow="3960" windowWidth="28660" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Data/Output_BE</t>
+  </si>
+  <si>
+    <t>RPATestingGetOrdersBot</t>
   </si>
 </sst>
 </file>
@@ -597,50 +597,50 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1697,18 +1697,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1732,7 +1732,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1754,7 +1754,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1765,7 +1765,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1776,53 +1776,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2824,7 +2824,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>